<commit_message>
maj de la Part_List_RISM.xlsx
</commit_message>
<xml_diff>
--- a/KiCad/2012_HypnoZ/Part_List_RISM.xlsx
+++ b/KiCad/2012_HypnoZ/Part_List_RISM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>C1</t>
   </si>
@@ -304,6 +304,66 @@
   </si>
   <si>
     <t>U1,U2,U3,U4</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>C2,C4</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>RELAIS-DPDT</t>
+  </si>
+  <si>
+    <t>FET_N</t>
+  </si>
+  <si>
+    <t>LM7805</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>D1,D2,D3</t>
+  </si>
+  <si>
+    <t>DIODE ?R3</t>
+  </si>
+  <si>
+    <t>Carte contacteur</t>
+  </si>
+  <si>
+    <t>K1,K2,K3</t>
+  </si>
+  <si>
+    <t>Relais</t>
+  </si>
+  <si>
+    <t>Bornier 4</t>
+  </si>
+  <si>
+    <t>Q1,Q2,Q3</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>R3,R5,R7</t>
+  </si>
+  <si>
+    <t>R4,R6,R8</t>
+  </si>
+  <si>
+    <t>220ohm 0,25W</t>
+  </si>
+  <si>
+    <t>Logique</t>
   </si>
 </sst>
 </file>
@@ -347,12 +407,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I55"/>
+  <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1284,7 +1347,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -1298,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -1326,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1340,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -1354,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1368,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -1380,6 +1443,236 @@
       </c>
       <c r="F55">
         <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="B58" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" t="s">
+        <v>29</v>
+      </c>
+      <c r="I59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+      <c r="E60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" t="s">
+        <v>100</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+      <c r="E64" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" t="s">
+        <v>106</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" s="3">
+        <v>4001</v>
+      </c>
+      <c r="E73" t="s">
+        <v>99</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>